<commit_message>
added total heatmap generation
</commit_message>
<xml_diff>
--- a/REyeker-DataAnalyses-Python/data/aoi_categorized/AOI_BI_BubbleSort.xlsx
+++ b/REyeker-DataAnalyses-Python/data/aoi_categorized/AOI_BI_BubbleSort.xlsx
@@ -14,7 +14,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1</t>
+  </si>
   <si>
     <t>startHeight</t>
   </si>
@@ -401,316 +419,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>30</v>
       </c>
-      <c r="B2">
+      <c r="I2">
         <v>57</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>688</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>688</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>58</v>
+      </c>
+      <c r="I3">
+        <v>85</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>688</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>86</v>
+      </c>
+      <c r="I4">
+        <v>113</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>688</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>114</v>
+      </c>
+      <c r="I5">
+        <v>141</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>688</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>142</v>
+      </c>
+      <c r="I6">
+        <v>169</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>688</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>58</v>
-      </c>
-      <c r="B3">
-        <v>85</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>688</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>86</v>
-      </c>
-      <c r="B4">
-        <v>113</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>688</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>114</v>
-      </c>
-      <c r="B5">
-        <v>141</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>688</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D7">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>142</v>
-      </c>
-      <c r="B6">
-        <v>169</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>688</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E7">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
         <v>226</v>
       </c>
-      <c r="B7">
+      <c r="I7">
         <v>253</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>688</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>688</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
         <v>254</v>
       </c>
-      <c r="B8">
+      <c r="I8">
         <v>281</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>688</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>688</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
         <v>282</v>
       </c>
-      <c r="B9">
+      <c r="I9">
         <v>309</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>688</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>688</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
         <v>310</v>
       </c>
-      <c r="B10">
+      <c r="I10">
         <v>337</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>688</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>688</v>
+      </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
         <v>338</v>
       </c>
-      <c r="B11">
+      <c r="I11">
         <v>365</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>688</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>688</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
         <v>366</v>
       </c>
-      <c r="B12">
+      <c r="I12">
         <v>393</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>688</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>688</v>
+      </c>
+      <c r="L12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
         <v>394</v>
       </c>
-      <c r="B13">
+      <c r="I13">
         <v>421</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>688</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>688</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
         <v>422</v>
       </c>
-      <c r="B14">
+      <c r="I14">
         <v>449</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>688</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>688</v>
+      </c>
+      <c r="L14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
         <v>450</v>
       </c>
-      <c r="B15">
+      <c r="I15">
         <v>477</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>688</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>688</v>
+      </c>
+      <c r="L15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16">
         <v>478</v>
       </c>
-      <c r="B16">
+      <c r="I16">
         <v>505</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>688</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>688</v>
+      </c>
+      <c r="L16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
         <v>506</v>
       </c>
-      <c r="B17">
+      <c r="I17">
         <v>533</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>688</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>688</v>
+      </c>
+      <c r="L17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18">
         <v>534</v>
       </c>
-      <c r="B18">
+      <c r="I18">
         <v>561</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>688</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>688</v>
+      </c>
+      <c r="L18" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>